<commit_message>
added space before stupid excel date format
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49243F7C-51A3-134B-A8C7-872BC4AA4D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D283225-F998-E745-8F65-AC36927F7753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36980" yWindow="740" windowWidth="20360" windowHeight="19020" xr2:uid="{8E2BECA6-270F-C740-9ED5-1344B6EDB180}"/>
+    <workbookView xWindow="-36200" yWindow="520" windowWidth="25860" windowHeight="19060" xr2:uid="{8E2BECA6-270F-C740-9ED5-1344B6EDB180}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="51">
   <si>
     <t>week_start</t>
   </si>
@@ -171,6 +171,24 @@
   </si>
   <si>
     <t>TBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-11</t>
   </si>
 </sst>
 </file>
@@ -542,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFD2179-9860-BE4A-AB2A-CF760AB84B2E}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1358,8 +1376,8 @@
       <c r="C52" s="1">
         <v>45546</v>
       </c>
-      <c r="E52" s="2">
-        <v>45171</v>
+      <c r="E52" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="G52" t="s">
         <v>13</v>
@@ -1395,8 +1413,8 @@
       <c r="D54" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="1">
-        <v>45194</v>
+      <c r="E54" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="H54" t="s">
         <v>21</v>
@@ -1457,8 +1475,8 @@
       <c r="D58" t="s">
         <v>4</v>
       </c>
-      <c r="E58" s="1">
-        <v>45222</v>
+      <c r="E58" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H58" t="s">
         <v>24</v>
@@ -1488,8 +1506,8 @@
       <c r="C60" s="1">
         <v>45604</v>
       </c>
-      <c r="E60" s="1">
-        <v>45240</v>
+      <c r="E60" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="G60" t="s">
         <v>14</v>
@@ -1525,8 +1543,8 @@
       <c r="D62" t="s">
         <v>5</v>
       </c>
-      <c r="E62" s="1">
-        <v>45616</v>
+      <c r="E62" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="H62" t="s">
         <v>28</v>
@@ -1542,8 +1560,8 @@
       <c r="C63" s="1">
         <v>45628</v>
       </c>
-      <c r="E63" s="1">
-        <v>45258</v>
+      <c r="E63" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="G63" t="s">
         <v>15</v>

</xml_diff>